<commit_message>
Test Data changes - Companies module - 4th Dec 2023
</commit_message>
<xml_diff>
--- a/TestData/T1174_Companies_AddCFOpportunityOnCompanyDetailPage.xlsx
+++ b/TestData/T1174_Companies_AddCFOpportunityOnCompanyDetailPage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C1E600-646D-4D1A-8601-0CF00F176223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87D8BFF-6B1C-4148-9F78-ACE53264AFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,7 +176,7 @@
     <t>BUS</t>
   </si>
   <si>
-    <t>Drew Koecher</t>
+    <t>Ayati Arvind</t>
   </si>
 </sst>
 </file>
@@ -744,7 +744,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Changes 15 May 2024
</commit_message>
<xml_diff>
--- a/TestData/T1174_Companies_AddCFOpportunityOnCompanyDetailPage.xlsx
+++ b/TestData/T1174_Companies_AddCFOpportunityOnCompanyDetailPage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87D8BFF-6B1C-4148-9F78-ACE53264AFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19801C17-75D2-4A27-83B8-983D9B5CD8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23040" windowHeight="11292" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>StdUser</t>
   </si>
   <si>
-    <t>Sector</t>
-  </si>
-  <si>
     <t>Staff</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>AddOpportunity</t>
   </si>
   <si>
-    <t>Dealership &amp; Rental Services</t>
-  </si>
-  <si>
     <t>Accountant</t>
   </si>
   <si>
@@ -177,6 +171,12 @@
   </si>
   <si>
     <t>Ayati Arvind</t>
+  </si>
+  <si>
+    <t>HL Sector ID</t>
+  </si>
+  <si>
+    <t>CSDN-0000001546</t>
   </si>
 </sst>
 </file>
@@ -560,10 +560,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,10 +605,10 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>14</v>
@@ -617,34 +617,34 @@
         <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>12</v>
@@ -653,19 +653,19 @@
         <v>10</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -676,13 +676,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -691,7 +691,7 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
@@ -706,10 +706,10 @@
         <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O2" t="s">
         <v>13</v>
@@ -718,19 +718,19 @@
         <v>11</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" t="s">
         <v>43</v>
       </c>
-      <c r="S2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" t="s">
-        <v>45</v>
-      </c>
       <c r="U2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -743,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -761,7 +761,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>